<commit_message>
Tarea 12 - 1ª mitad
</commit_message>
<xml_diff>
--- a/controlDedicacion.xlsx
+++ b/controlDedicacion.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
   <si>
     <t xml:space="preserve">NIP del estudiante:</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tarea 11, el añadido a tarea 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tareas 12 y 13</t>
   </si>
   <si>
     <t xml:space="preserve">Tiempo total dedicado    </t>
@@ -524,18 +527,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:L38"/>
+  <dimension ref="B2:L45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="3.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.81"/>
@@ -1084,39 +1088,51 @@
     </row>
     <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
+      <c r="C25" s="11" t="n">
+        <v>30</v>
+      </c>
       <c r="D25" s="12" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(C25/60)</f>
         <v>0</v>
       </c>
       <c r="E25" s="12" t="n">
         <f aca="false">MOD(C25,60)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F25" s="12" t="str">
         <f aca="false">_xlfn.CONCAT(IF(D25=0, "", _xlfn.CONCAT(D25, "h")), IF(E25=0, "", _xlfn.CONCAT(E25, "min")))</f>
-        <v/>
-      </c>
-      <c r="G25" s="12"/>
-      <c r="H25" s="13"/>
+        <v>30min</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
+      <c r="C26" s="11" t="n">
+        <v>45</v>
+      </c>
       <c r="D26" s="12" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(C26/60)</f>
         <v>0</v>
       </c>
       <c r="E26" s="12" t="n">
         <f aca="false">MOD(C26,60)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="F26" s="12" t="str">
         <f aca="false">_xlfn.CONCAT(IF(D26=0, "", _xlfn.CONCAT(D26, "h")), IF(E26=0, "", _xlfn.CONCAT(E26, "min")))</f>
-        <v/>
-      </c>
-      <c r="G26" s="12"/>
-      <c r="H26" s="13"/>
+        <v>45min</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="11"/>
@@ -1154,9 +1170,9 @@
       <c r="G28" s="12"/>
       <c r="H28" s="13"/>
     </row>
-    <row r="29" customFormat="false" ht="16.4" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
+    <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
       <c r="D29" s="12" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(C29/60)</f>
         <v>0</v>
@@ -1165,92 +1181,218 @@
         <f aca="false">MOD(C29,60)</f>
         <v>0</v>
       </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="17"/>
-    </row>
-    <row r="30" customFormat="false" ht="16.4" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="15"/>
-      <c r="C30" s="15" t="n">
-        <f aca="false">SUM(C6:C29)</f>
-        <v>705</v>
-      </c>
+      <c r="F29" s="12" t="str">
+        <f aca="false">_xlfn.CONCAT(IF(D29=0, "", _xlfn.CONCAT(D29, "h")), IF(E29=0, "", _xlfn.CONCAT(E29, "min")))</f>
+        <v/>
+      </c>
+      <c r="G29" s="12"/>
+      <c r="H29" s="13"/>
+    </row>
+    <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
       <c r="D30" s="12" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(C30/60)</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E30" s="12" t="n">
         <f aca="false">MOD(C30,60)</f>
-        <v>45</v>
-      </c>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="17"/>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="19" t="str">
-        <f aca="false">_xlfn.CONCAT(IF(D30=0, "", _xlfn.CONCAT(D30, "h")),, IF(E30=0, "", _xlfn.CONCAT(E30, "min")))</f>
-        <v>11h45min</v>
-      </c>
-      <c r="H31" s="20"/>
-    </row>
-    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="12" t="str">
+        <f aca="false">_xlfn.CONCAT(IF(D30=0, "", _xlfn.CONCAT(D30, "h")), IF(E30=0, "", _xlfn.CONCAT(E30, "min")))</f>
+        <v/>
+      </c>
+      <c r="G30" s="12"/>
+      <c r="H30" s="13"/>
+    </row>
+    <row r="31" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="12" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH(C31/60)</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="12" t="n">
+        <f aca="false">MOD(C31,60)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="12" t="str">
+        <f aca="false">_xlfn.CONCAT(IF(D31=0, "", _xlfn.CONCAT(D31, "h")), IF(E31=0, "", _xlfn.CONCAT(E31, "min")))</f>
+        <v/>
+      </c>
+      <c r="G31" s="12"/>
+      <c r="H31" s="13"/>
+    </row>
+    <row r="32" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="12" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH(C32/60)</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="12" t="n">
+        <f aca="false">MOD(C32,60)</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="12" t="str">
+        <f aca="false">_xlfn.CONCAT(IF(D32=0, "", _xlfn.CONCAT(D32, "h")), IF(E32=0, "", _xlfn.CONCAT(E32, "min")))</f>
+        <v/>
+      </c>
+      <c r="G32" s="12"/>
+      <c r="H32" s="13"/>
+    </row>
+    <row r="33" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="12" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH(C33/60)</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="12" t="n">
+        <f aca="false">MOD(C33,60)</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="12" t="str">
+        <f aca="false">_xlfn.CONCAT(IF(D33=0, "", _xlfn.CONCAT(D33, "h")), IF(E33=0, "", _xlfn.CONCAT(E33, "min")))</f>
+        <v/>
+      </c>
+      <c r="G33" s="12"/>
+      <c r="H33" s="13"/>
+    </row>
+    <row r="34" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="12" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH(C34/60)</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="12" t="n">
+        <f aca="false">MOD(C34,60)</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="12" t="str">
+        <f aca="false">_xlfn.CONCAT(IF(D34=0, "", _xlfn.CONCAT(D34, "h")), IF(E34=0, "", _xlfn.CONCAT(E34, "min")))</f>
+        <v/>
+      </c>
+      <c r="G34" s="12"/>
+      <c r="H34" s="13"/>
+    </row>
+    <row r="35" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="12" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH(C35/60)</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="12" t="n">
+        <f aca="false">MOD(C35,60)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="12" t="str">
+        <f aca="false">_xlfn.CONCAT(IF(D35=0, "", _xlfn.CONCAT(D35, "h")), IF(E35=0, "", _xlfn.CONCAT(E35, "min")))</f>
+        <v/>
+      </c>
+      <c r="G35" s="12"/>
+      <c r="H35" s="13"/>
+    </row>
+    <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="12" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH(C36/60)</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="12" t="n">
+        <f aca="false">MOD(C36,60)</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="17"/>
+    </row>
+    <row r="37" customFormat="false" ht="16.4" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B37" s="15"/>
+      <c r="C37" s="15" t="n">
+        <f aca="false">SUM(C6:C36)</f>
+        <v>780</v>
+      </c>
+      <c r="D37" s="12" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH(C37/60)</f>
+        <v>13</v>
+      </c>
+      <c r="E37" s="12" t="n">
+        <f aca="false">MOD(C37,60)</f>
+        <v>0</v>
+      </c>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="17"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-    </row>
-    <row r="35" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="22" t="s">
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="19" t="str">
+        <f aca="false">_xlfn.CONCAT(IF(D37=0, "", _xlfn.CONCAT(D37, "h")),, IF(E37=0, "", _xlfn.CONCAT(E37, "min")))</f>
+        <v>13h</v>
+      </c>
+      <c r="H38" s="20"/>
+    </row>
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="22"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-    </row>
-    <row r="37" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="22" t="s">
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+    </row>
+    <row r="42" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B42" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+    </row>
+    <row r="44" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B44" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -1265,10 +1407,10 @@
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B35:H36"/>
-    <mergeCell ref="B37:H38"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B42:H43"/>
+    <mergeCell ref="B44:H45"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Preparar clase Tag para la entrega
</commit_message>
<xml_diff>
--- a/controlDedicacion.xlsx
+++ b/controlDedicacion.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
   <si>
     <t xml:space="preserve">NIP del estudiante:</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t xml:space="preserve">Tareas 12 y 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarea 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preparar archivos para entrega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tareas 11 y 12</t>
   </si>
   <si>
     <t xml:space="preserve">Tiempo total dedicado    </t>
@@ -529,8 +538,8 @@
   </sheetPr>
   <dimension ref="B2:L45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1113,19 +1122,19 @@
     <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="11"/>
       <c r="C26" s="11" t="n">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D26" s="12" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(C26/60)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="12" t="n">
         <f aca="false">MOD(C26,60)</f>
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F26" s="12" t="str">
         <f aca="false">_xlfn.CONCAT(IF(D26=0, "", _xlfn.CONCAT(D26, "h")), IF(E26=0, "", _xlfn.CONCAT(E26, "min")))</f>
-        <v>45min</v>
+        <v>1h</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>12</v>
@@ -1136,57 +1145,75 @@
     </row>
     <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
+      <c r="C27" s="11" t="n">
+        <v>15</v>
+      </c>
       <c r="D27" s="12" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(C27/60)</f>
         <v>0</v>
       </c>
       <c r="E27" s="12" t="n">
         <f aca="false">MOD(C27,60)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F27" s="12" t="str">
         <f aca="false">_xlfn.CONCAT(IF(D27=0, "", _xlfn.CONCAT(D27, "h")), IF(E27=0, "", _xlfn.CONCAT(E27, "min")))</f>
-        <v/>
-      </c>
-      <c r="G27" s="12"/>
-      <c r="H27" s="13"/>
+        <v>15min</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
+      <c r="C28" s="11" t="n">
+        <v>15</v>
+      </c>
       <c r="D28" s="12" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(C28/60)</f>
         <v>0</v>
       </c>
       <c r="E28" s="12" t="n">
         <f aca="false">MOD(C28,60)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F28" s="12" t="str">
         <f aca="false">_xlfn.CONCAT(IF(D28=0, "", _xlfn.CONCAT(D28, "h")), IF(E28=0, "", _xlfn.CONCAT(E28, "min")))</f>
-        <v/>
-      </c>
-      <c r="G28" s="12"/>
-      <c r="H28" s="13"/>
+        <v>15min</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
+      <c r="C29" s="11" t="n">
+        <v>15</v>
+      </c>
       <c r="D29" s="12" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(C29/60)</f>
         <v>0</v>
       </c>
       <c r="E29" s="12" t="n">
         <f aca="false">MOD(C29,60)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F29" s="12" t="str">
         <f aca="false">_xlfn.CONCAT(IF(D29=0, "", _xlfn.CONCAT(D29, "h")), IF(E29=0, "", _xlfn.CONCAT(E29, "min")))</f>
-        <v/>
-      </c>
-      <c r="G29" s="12"/>
-      <c r="H29" s="13"/>
+        <v>15min</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="11"/>
@@ -1315,11 +1342,11 @@
       <c r="B37" s="15"/>
       <c r="C37" s="15" t="n">
         <f aca="false">SUM(C6:C36)</f>
-        <v>780</v>
+        <v>840</v>
       </c>
       <c r="D37" s="12" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(C37/60)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E37" s="12" t="n">
         <f aca="false">MOD(C37,60)</f>
@@ -1331,7 +1358,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="18" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="18"/>
@@ -1339,13 +1366,13 @@
       <c r="F38" s="18"/>
       <c r="G38" s="19" t="str">
         <f aca="false">_xlfn.CONCAT(IF(D37=0, "", _xlfn.CONCAT(D37, "h")),, IF(E37=0, "", _xlfn.CONCAT(E37, "min")))</f>
-        <v>13h</v>
+        <v>14h</v>
       </c>
       <c r="H38" s="20"/>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="21" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="21"/>
@@ -1356,7 +1383,7 @@
     </row>
     <row r="42" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B42" s="22" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C42" s="22"/>
       <c r="D42" s="22"/>
@@ -1376,7 +1403,7 @@
     </row>
     <row r="44" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="22" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C44" s="22"/>
       <c r="D44" s="22"/>

</xml_diff>